<commit_message>
"New Changes done on the Data Driven part. Add multiple data sets"
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BusBookingData.xlsx
+++ b/src/test/resources/testdata/BusBookingData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\MakeMyTrip\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1BEF97-D44D-41F3-9417-B40FC91C1F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0C342B-ABD0-4E38-BFAA-0CE0BDC83295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BusData" sheetId="1" r:id="rId1"/>
+    <sheet name="BusBookingData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>fromCity</t>
   </si>
@@ -43,13 +43,127 @@
   </si>
   <si>
     <t>Aug 22 2025</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>vijaysjofficial@gmail.com</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>9994050623</t>
+  </si>
+  <si>
+    <t>Chidambaram, Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Aug 26 2025</t>
+  </si>
+  <si>
+    <t>ajayrajendran@gmail.com</t>
+  </si>
+  <si>
+    <t>7395950623</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>From Chennai to Salem</t>
+  </si>
+  <si>
+    <t>From Chennai to Chidambaram</t>
+  </si>
+  <si>
+    <t>Manimegalai</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Vidhya</t>
+  </si>
+  <si>
+    <t>manimegalai@gmail.com</t>
+  </si>
+  <si>
+    <t>7395950624</t>
+  </si>
+  <si>
+    <t>7395950625</t>
+  </si>
+  <si>
+    <t>Swathi</t>
+  </si>
+  <si>
+    <t>vidhyadevi@gmail.com</t>
+  </si>
+  <si>
+    <t>swathi@gmail.com</t>
+  </si>
+  <si>
+    <t>7395950626</t>
+  </si>
+  <si>
+    <t>From Chennai to Mayiladuthurai</t>
+  </si>
+  <si>
+    <t>From Chennai to Karur</t>
+  </si>
+  <si>
+    <t>From Chennai to Thiruvarur</t>
+  </si>
+  <si>
+    <t>Karur, Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Thiruvarur, Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Vijay</t>
+  </si>
+  <si>
+    <t>Ajay</t>
+  </si>
+  <si>
+    <t>Aug 28 2025</t>
+  </si>
+  <si>
+    <t>Aug 24 2025</t>
+  </si>
+  <si>
+    <t>Aug 30 2025</t>
+  </si>
+  <si>
+    <t>Karaikal, Tamil Nadu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,13 +179,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,22 +217,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,40 +526,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="5">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="5">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5">
+        <v>29</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5">
+        <v>29</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{04335AB9-1502-4CED-A044-1756A0ADF133}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{33BABA04-5DF3-4BDD-BEBD-9A7F8D298D7A}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{6C9B72BE-49A1-49E8-AE50-376BD24311BB}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{8314973C-8624-472C-9EEF-FD722EB191CF}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{6E63F659-A4F7-4B15-8C4D-5ACA7C3BCEDA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes done in FrameworkConstants
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BusBookingData.xlsx
+++ b/src/test/resources/testdata/BusBookingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\MakeMyTrip\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0C342B-ABD0-4E38-BFAA-0CE0BDC83295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981CED38-2079-472C-B402-25903C24F0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,9 +126,6 @@
     <t>7395950626</t>
   </si>
   <si>
-    <t>From Chennai to Mayiladuthurai</t>
-  </si>
-  <si>
     <t>From Chennai to Karur</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Karaikal, Tamil Nadu</t>
+  </si>
+  <si>
+    <t>From Chennai to Karaikal</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -592,7 +592,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="5">
         <v>27</v>
@@ -612,19 +612,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="5">
         <v>27</v>
@@ -644,13 +644,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -685,7 +685,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>25</v>
@@ -708,16 +708,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>29</v>

</xml_diff>